<commit_message>
Corregido bug en sh_fases.py
</commit_message>
<xml_diff>
--- a/files/SHAMPOO COLAGENO.xlsx
+++ b/files/SHAMPOO COLAGENO.xlsx
@@ -137,37 +137,37 @@
     <t xml:space="preserve">0862</t>
   </si>
   <si>
+    <t xml:space="preserve">SAV CLG SHFCO 12X550 EAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0997</t>
+  </si>
+  <si>
     <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAV CLG SHFCO 12X550 EAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10000919</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0158</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0159</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0997</t>
   </si>
   <si>
     <t xml:space="preserve">0161</t>
@@ -412,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -466,6 +466,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,7 +572,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="R3" activeCellId="0" sqref="R3:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -756,7 +760,7 @@
       <c r="Q3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -812,7 +816,7 @@
       <c r="Q4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -868,7 +872,7 @@
       <c r="Q5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -924,7 +928,7 @@
       <c r="Q6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -980,8 +984,8 @@
       <c r="Q7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="13" t="s">
-        <v>38</v>
+      <c r="R7" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -989,13 +993,13 @@
         <v>43211</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>43202</v>
@@ -1034,10 +1038,10 @@
         <v>550</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1045,13 +1049,13 @@
         <v>43211</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>43203</v>
@@ -1090,10 +1094,10 @@
         <v>550</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1101,13 +1105,13 @@
         <v>43211</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>43203</v>
@@ -1146,10 +1150,10 @@
         <v>550</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1157,13 +1161,13 @@
         <v>43211</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>43204</v>
@@ -1202,10 +1206,10 @@
         <v>550</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1261,7 +1265,7 @@
         <v>50</v>
       </c>
       <c r="R12" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1317,7 +1321,7 @@
         <v>52</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1373,7 +1377,7 @@
         <v>54</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1429,7 +1433,7 @@
         <v>56</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1485,7 +1489,7 @@
         <v>58</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1541,7 +1545,7 @@
         <v>60</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1549,10 +1553,10 @@
         <v>43236</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>61</v>
@@ -1597,7 +1601,7 @@
         <v>62</v>
       </c>
       <c r="R18" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1605,10 +1609,10 @@
         <v>43236</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>63</v>
@@ -1653,7 +1657,7 @@
         <v>64</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1661,10 +1665,10 @@
         <v>43236</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
@@ -1709,7 +1713,7 @@
         <v>66</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1717,10 +1721,10 @@
         <v>43236</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>67</v>
@@ -1765,7 +1769,7 @@
         <v>68</v>
       </c>
       <c r="R21" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1773,10 +1777,10 @@
         <v>43236</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>69</v>
@@ -1821,7 +1825,7 @@
         <v>70</v>
       </c>
       <c r="R22" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1829,10 +1833,10 @@
         <v>43236</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>71</v>
@@ -1877,7 +1881,7 @@
         <v>72</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1885,10 +1889,10 @@
         <v>43236</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>73</v>
@@ -1933,7 +1937,7 @@
         <v>74</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1941,10 +1945,10 @@
         <v>43236</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>75</v>
@@ -1989,7 +1993,7 @@
         <v>76</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1997,10 +2001,10 @@
         <v>43236</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>77</v>
@@ -2045,7 +2049,7 @@
         <v>78</v>
       </c>
       <c r="R26" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2053,10 +2057,10 @@
         <v>43236</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>79</v>
@@ -2101,7 +2105,7 @@
         <v>80</v>
       </c>
       <c r="R27" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2109,10 +2113,10 @@
         <v>43236</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>81</v>
@@ -2157,7 +2161,7 @@
         <v>82</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2165,10 +2169,10 @@
         <v>43236</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>83</v>
@@ -2213,7 +2217,7 @@
         <v>84</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2221,10 +2225,10 @@
         <v>43236</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>85</v>
@@ -2269,7 +2273,7 @@
         <v>86</v>
       </c>
       <c r="R30" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2277,10 +2281,10 @@
         <v>43236</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>87</v>
@@ -2325,7 +2329,7 @@
         <v>88</v>
       </c>
       <c r="R31" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2333,10 +2337,10 @@
         <v>43236</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>89</v>
@@ -2381,7 +2385,7 @@
         <v>90</v>
       </c>
       <c r="R32" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2389,10 +2393,10 @@
         <v>43242</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>91</v>
@@ -2437,7 +2441,7 @@
         <v>92</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2445,10 +2449,10 @@
         <v>43242</v>
       </c>
       <c r="B34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>93</v>
@@ -2493,7 +2497,7 @@
         <v>94</v>
       </c>
       <c r="R34" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2549,7 +2553,7 @@
         <v>96</v>
       </c>
       <c r="R35" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2605,7 +2609,7 @@
         <v>98</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2631,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2657,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="R38" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2683,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="R39" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2709,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="R40" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2735,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="R41" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2761,7 +2765,7 @@
         <v>0</v>
       </c>
       <c r="R42" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2787,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="R43" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2813,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="R44" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2839,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="R45" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2865,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="R46" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2891,7 +2895,7 @@
         <v>0</v>
       </c>
       <c r="R47" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2917,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="R48" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2943,7 +2947,7 @@
         <v>0</v>
       </c>
       <c r="R49" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2969,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2995,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3021,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="R52" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3047,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="R53" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3073,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="R54" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3099,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="R55" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3125,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="R56" s="13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3170,7 +3174,7 @@
   <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="R3:R10 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3182,7 +3186,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>10000919</v>

</xml_diff>

<commit_message>
WIP pdf_creatiom.py - 4
</commit_message>
<xml_diff>
--- a/files/SHAMPOO COLAGENO.xlsx
+++ b/files/SHAMPOO COLAGENO.xlsx
@@ -1,361 +1,385 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8190" windowWidth="16380" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SH. COLAGENO" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SH. COLAGENO" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
-  <si>
-    <t>Fecha de edición</t>
-  </si>
-  <si>
-    <t>ReferenciaQ</t>
-  </si>
-  <si>
-    <t>CódigoQ</t>
-  </si>
-  <si>
-    <t>LoteQV</t>
-  </si>
-  <si>
-    <t>FEQ</t>
-  </si>
-  <si>
-    <t>FVQ</t>
-  </si>
-  <si>
-    <t>CajasQV</t>
-  </si>
-  <si>
-    <t>u_cajaQ</t>
-  </si>
-  <si>
-    <t>Total_uQ</t>
-  </si>
-  <si>
-    <t>AspectoQ</t>
-  </si>
-  <si>
-    <t>Rango pHQ</t>
-  </si>
-  <si>
-    <t>Resultado pHQV</t>
-  </si>
-  <si>
-    <t>Rango viscosidadQ</t>
-  </si>
-  <si>
-    <t>Resultado viscosidadQV</t>
-  </si>
-  <si>
-    <t>Rango peso netoQ</t>
-  </si>
-  <si>
-    <t>Resultado peso netoQ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="99">
+  <si>
+    <t xml:space="preserve">Fecha de edición</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReferenciaQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CódigoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoteQV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FVQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CajasQV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u_cajaQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_uQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AspectoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rango pHQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado pHQV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rango viscosidadQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado viscosidadQV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rango peso netoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado peso netoQ</t>
   </si>
   <si>
     <t xml:space="preserve">Consecutivo </t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>SAV CLG SHFCO 12X550</t>
-  </si>
-  <si>
-    <t>10000918</t>
-  </si>
-  <si>
-    <t>0131</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>MEZCLA HOMOGÉNEA PERLADA SIN PARTÍCULAS EN SUSPENSIÓN O GRUMOS</t>
-  </si>
-  <si>
-    <t>5,75-6,25</t>
-  </si>
-  <si>
-    <t>13000-17000</t>
-  </si>
-  <si>
-    <t>545,00-555,00</t>
-  </si>
-  <si>
-    <t>0772</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>0132</t>
-  </si>
-  <si>
-    <t>0773</t>
-  </si>
-  <si>
-    <t>0133</t>
-  </si>
-  <si>
-    <t>0774</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>0134</t>
-  </si>
-  <si>
-    <t>0775</t>
-  </si>
-  <si>
-    <t>0135</t>
-  </si>
-  <si>
-    <t>0861</t>
-  </si>
-  <si>
-    <t>0136</t>
-  </si>
-  <si>
-    <t>0862</t>
-  </si>
-  <si>
-    <t>SAV CLG SHFCO 12X550 EAN</t>
-  </si>
-  <si>
-    <t>10000919</t>
-  </si>
-  <si>
-    <t>0157</t>
-  </si>
-  <si>
-    <t>0994</t>
-  </si>
-  <si>
-    <t>0158</t>
-  </si>
-  <si>
-    <t>0995</t>
-  </si>
-  <si>
-    <t>0159</t>
-  </si>
-  <si>
-    <t>0996</t>
-  </si>
-  <si>
-    <t>0160</t>
-  </si>
-  <si>
-    <t>0997</t>
-  </si>
-  <si>
-    <t>0161</t>
-  </si>
-  <si>
-    <t>0998</t>
-  </si>
-  <si>
-    <t>0162</t>
-  </si>
-  <si>
-    <t>0999</t>
-  </si>
-  <si>
-    <t>0163</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>0164</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>0169</t>
-  </si>
-  <si>
-    <t>1004</t>
-  </si>
-  <si>
-    <t>0170</t>
-  </si>
-  <si>
-    <t>1005</t>
-  </si>
-  <si>
-    <t>0181</t>
-  </si>
-  <si>
-    <t>1035</t>
-  </si>
-  <si>
-    <t>0182</t>
-  </si>
-  <si>
-    <t>1036</t>
-  </si>
-  <si>
-    <t>0183</t>
-  </si>
-  <si>
-    <t>1037</t>
-  </si>
-  <si>
-    <t>0184</t>
-  </si>
-  <si>
-    <t>1038</t>
-  </si>
-  <si>
-    <t>0185</t>
-  </si>
-  <si>
-    <t>1039</t>
-  </si>
-  <si>
-    <t>0186</t>
-  </si>
-  <si>
-    <t>1040</t>
-  </si>
-  <si>
-    <t>0187</t>
-  </si>
-  <si>
-    <t>1041</t>
-  </si>
-  <si>
-    <t>0188</t>
-  </si>
-  <si>
-    <t>1042</t>
-  </si>
-  <si>
-    <t>0189</t>
-  </si>
-  <si>
-    <t>1043</t>
-  </si>
-  <si>
-    <t>0190</t>
-  </si>
-  <si>
-    <t>1044</t>
-  </si>
-  <si>
-    <t>0191</t>
-  </si>
-  <si>
-    <t>1045</t>
-  </si>
-  <si>
-    <t>0192</t>
-  </si>
-  <si>
-    <t>1046</t>
-  </si>
-  <si>
-    <t>0193</t>
-  </si>
-  <si>
-    <t>1047</t>
-  </si>
-  <si>
-    <t>0194</t>
-  </si>
-  <si>
-    <t>1048</t>
-  </si>
-  <si>
-    <t>0195</t>
-  </si>
-  <si>
-    <t>1049</t>
-  </si>
-  <si>
-    <t>0196</t>
-  </si>
-  <si>
-    <t>1087</t>
-  </si>
-  <si>
-    <t>0197</t>
-  </si>
-  <si>
-    <t>1088</t>
-  </si>
-  <si>
-    <t>0198</t>
-  </si>
-  <si>
-    <t>1089</t>
-  </si>
-  <si>
-    <t>0199</t>
-  </si>
-  <si>
-    <t>1090</t>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAV CLG SHFCO 12X550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEZCLA HOMOGÉNEA PERLADA SIN PARTÍCULAS EN SUSPENSIÓN O GRUMOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,75-6,25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13000-17000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">545,00-555,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0861</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAV CLG SHFCO 12X550 EAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1090</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="yyyy\-mm\-dd;@" numFmtId="164"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD;@"/>
+    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <u val="single"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -363,68 +387,102 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+  <cellXfs count="15">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -435,330 +493,110 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0" zoomScaleNormal="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A17" ySplit="1"/>
-      <selection activeCell="K1" sqref="K1"/>
-      <selection activeCell="R23" pane="bottomLeft" sqref="R23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="R4" activeCellId="0" sqref="R4:R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="13.7109375"/>
-    <col customWidth="1" max="2" min="2" style="2" width="39.28515625"/>
-    <col customWidth="1" max="3" min="3" style="2" width="10.5703125"/>
-    <col customWidth="1" max="4" min="4" style="3" width="11.42578125"/>
-    <col customWidth="1" max="6" min="5" style="1" width="11.42578125"/>
-    <col customWidth="1" max="7" min="7" style="4" width="11.42578125"/>
-    <col customWidth="1" max="9" min="8" style="2" width="10.5703125"/>
-    <col customWidth="1" max="10" min="10" style="2" width="86.5703125"/>
-    <col customWidth="1" max="11" min="11" style="2" width="16.42578125"/>
-    <col customWidth="1" max="12" min="12" style="4" width="11.42578125"/>
-    <col customWidth="1" max="13" min="13" style="2" width="15.42578125"/>
-    <col customWidth="1" max="14" min="14" style="4" width="13.7109375"/>
-    <col customWidth="1" max="15" min="15" style="2" width="16.7109375"/>
-    <col customWidth="1" max="16" min="16" style="5" width="12.85546875"/>
-    <col customWidth="1" max="17" min="17" style="3" width="15.28515625"/>
-    <col customWidth="1" max="18" min="18" style="3" width="24"/>
-    <col customWidth="1" max="1025" min="19" style="2" width="10.5703125"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="86.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="16.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="2" width="10.53"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="32.25" r="1" s="2" spans="1:18">
+    <row r="1" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -814,7 +652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="2" spans="1:18">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>43193</v>
       </c>
@@ -839,7 +677,7 @@
       <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -870,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="2" spans="1:18">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>43193</v>
       </c>
@@ -895,7 +733,7 @@
       <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -926,7 +764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="2" spans="1:18">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>43193</v>
       </c>
@@ -951,7 +789,7 @@
       <c r="H4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -978,11 +816,11 @@
       <c r="Q4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="5" s="2" spans="1:18">
+      <c r="R4" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>43193</v>
       </c>
@@ -1007,7 +845,7 @@
       <c r="H5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -1034,11 +872,11 @@
       <c r="Q5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="6" s="2" spans="1:18">
+      <c r="R5" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>43201</v>
       </c>
@@ -1063,7 +901,7 @@
       <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -1090,11 +928,11 @@
       <c r="Q6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="2" spans="1:18">
+      <c r="R6" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>43201</v>
       </c>
@@ -1119,7 +957,7 @@
       <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -1146,11 +984,11 @@
       <c r="Q7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="8" s="2" spans="1:18">
+      <c r="R7" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1175,7 +1013,7 @@
       <c r="H8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1202,11 +1040,11 @@
       <c r="Q8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="2" spans="1:18">
+      <c r="R8" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1231,7 +1069,7 @@
       <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J9" s="4" t="s">
@@ -1258,11 +1096,11 @@
       <c r="Q9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="10" s="2" spans="1:18">
+      <c r="R9" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1287,7 +1125,7 @@
       <c r="H10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -1314,11 +1152,11 @@
       <c r="Q10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="11" s="2" spans="1:18">
+      <c r="R10" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1343,7 +1181,7 @@
       <c r="H11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J11" s="4" t="s">
@@ -1370,11 +1208,11 @@
       <c r="Q11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="R11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="12" s="2" spans="1:18">
+      <c r="R11" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1399,7 +1237,7 @@
       <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J12" s="4" t="s">
@@ -1426,11 +1264,11 @@
       <c r="Q12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="13" s="2" spans="1:18">
+      <c r="R12" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1455,7 +1293,7 @@
       <c r="H13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1482,11 +1320,11 @@
       <c r="Q13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="R13" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="14" s="2" spans="1:18">
+      <c r="R13" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1511,7 +1349,7 @@
       <c r="H14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J14" s="4" t="s">
@@ -1538,11 +1376,11 @@
       <c r="Q14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="R14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="15" s="2" spans="1:18">
+      <c r="R14" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>43211</v>
       </c>
@@ -1567,7 +1405,7 @@
       <c r="H15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -1594,11 +1432,11 @@
       <c r="Q15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="16" s="2" spans="1:18">
+      <c r="R15" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>43222</v>
       </c>
@@ -1623,7 +1461,7 @@
       <c r="H16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J16" s="4" t="s">
@@ -1650,11 +1488,11 @@
       <c r="Q16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="17" s="2" spans="1:18">
+      <c r="R16" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>43222</v>
       </c>
@@ -1679,7 +1517,7 @@
       <c r="H17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J17" s="4" t="s">
@@ -1706,11 +1544,11 @@
       <c r="Q17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="18" s="2" spans="1:18">
+      <c r="R17" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>43236</v>
       </c>
@@ -1735,7 +1573,7 @@
       <c r="H18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J18" s="4" t="s">
@@ -1762,11 +1600,11 @@
       <c r="Q18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="R18" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="19" s="2" spans="1:18">
+      <c r="R18" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>43236</v>
       </c>
@@ -1791,7 +1629,7 @@
       <c r="H19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J19" s="4" t="s">
@@ -1818,11 +1656,11 @@
       <c r="Q19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="20" s="2" spans="1:18">
+      <c r="R19" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>43236</v>
       </c>
@@ -1847,7 +1685,7 @@
       <c r="H20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J20" s="4" t="s">
@@ -1874,11 +1712,11 @@
       <c r="Q20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R20" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="21" s="2" spans="1:18">
+      <c r="R20" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>43236</v>
       </c>
@@ -1903,7 +1741,7 @@
       <c r="H21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J21" s="4" t="s">
@@ -1930,11 +1768,11 @@
       <c r="Q21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="R21" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="22" s="2" spans="1:18">
+      <c r="R21" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>43236</v>
       </c>
@@ -1959,7 +1797,7 @@
       <c r="H22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J22" s="4" t="s">
@@ -1986,11 +1824,11 @@
       <c r="Q22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R22" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="23" s="2" spans="1:18">
+      <c r="R22" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2015,7 +1853,7 @@
       <c r="H23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J23" s="4" t="s">
@@ -2042,11 +1880,11 @@
       <c r="Q23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R23" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="24" s="2" spans="1:18">
+      <c r="R23" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2071,7 +1909,7 @@
       <c r="H24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J24" s="4" t="s">
@@ -2098,11 +1936,11 @@
       <c r="Q24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R24" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="25" s="2" spans="1:18">
+      <c r="R24" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2127,7 +1965,7 @@
       <c r="H25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -2154,11 +1992,11 @@
       <c r="Q25" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="R25" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="26" s="2" spans="1:18">
+      <c r="R25" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2183,7 +2021,7 @@
       <c r="H26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J26" s="4" t="s">
@@ -2210,11 +2048,11 @@
       <c r="Q26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R26" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="27" s="2" spans="1:18">
+      <c r="R26" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2239,7 +2077,7 @@
       <c r="H27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J27" s="4" t="s">
@@ -2266,11 +2104,11 @@
       <c r="Q27" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R27" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="28" s="2" spans="1:18">
+      <c r="R27" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2295,7 +2133,7 @@
       <c r="H28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I28" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J28" s="4" t="s">
@@ -2322,11 +2160,11 @@
       <c r="Q28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="R28" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="29" s="2" spans="1:18">
+      <c r="R28" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2351,7 +2189,7 @@
       <c r="H29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I29" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J29" s="4" t="s">
@@ -2378,11 +2216,11 @@
       <c r="Q29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R29" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="30" s="2" spans="1:18">
+      <c r="R29" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2407,7 +2245,7 @@
       <c r="H30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J30" s="4" t="s">
@@ -2434,11 +2272,11 @@
       <c r="Q30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="R30" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="31" s="2" spans="1:18">
+      <c r="R30" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2463,7 +2301,7 @@
       <c r="H31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J31" s="4" t="s">
@@ -2490,11 +2328,11 @@
       <c r="Q31" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="R31" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="32" s="2" spans="1:18">
+      <c r="R31" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>43236</v>
       </c>
@@ -2519,7 +2357,7 @@
       <c r="H32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J32" s="4" t="s">
@@ -2546,11 +2384,11 @@
       <c r="Q32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R32" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="33" s="2" spans="1:18">
+      <c r="R32" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>43242</v>
       </c>
@@ -2575,7 +2413,7 @@
       <c r="H33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I33" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J33" s="4" t="s">
@@ -2602,11 +2440,11 @@
       <c r="Q33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="R33" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="34" s="2" spans="1:18">
+      <c r="R33" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>43242</v>
       </c>
@@ -2631,7 +2469,7 @@
       <c r="H34" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J34" s="4" t="s">
@@ -2658,11 +2496,11 @@
       <c r="Q34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="R34" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="35" s="2" spans="1:18">
+      <c r="R34" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>43242</v>
       </c>
@@ -2687,7 +2525,7 @@
       <c r="H35" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35" s="2" t="n">
         <v>5460</v>
       </c>
       <c r="J35" s="4" t="s">
@@ -2714,11 +2552,11 @@
       <c r="Q35" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="R35" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.85" r="36" s="2" spans="1:18">
+      <c r="R35" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>43242</v>
       </c>
@@ -2743,7 +2581,7 @@
       <c r="H36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I36" s="2" t="n">
         <v>5376</v>
       </c>
       <c r="J36" s="4" t="s">
@@ -2770,18 +2608,18 @@
       <c r="Q36" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="R36" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="37" s="2" spans="1:18">
+      <c r="R36" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C37" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J37" s="4" t="n">
@@ -2796,18 +2634,18 @@
       <c r="O37" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R37" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="38" s="2" spans="1:18">
+      <c r="R37" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C38" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I38" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J38" s="4" t="n">
@@ -2822,18 +2660,18 @@
       <c r="O38" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R38" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="39" s="2" spans="1:18">
+      <c r="R38" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J39" s="4" t="n">
@@ -2848,18 +2686,18 @@
       <c r="O39" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R39" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="40" s="2" spans="1:18">
+      <c r="R39" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C40" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J40" s="4" t="n">
@@ -2874,18 +2712,18 @@
       <c r="O40" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R40" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="41" s="2" spans="1:18">
+      <c r="R40" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I41" t="n">
+      <c r="I41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J41" s="4" t="n">
@@ -2900,18 +2738,18 @@
       <c r="O41" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R41" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="42" s="2" spans="1:18">
+      <c r="R41" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H42" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I42" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J42" s="4" t="n">
@@ -2926,18 +2764,18 @@
       <c r="O42" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R42" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="43" s="2" spans="1:18">
+      <c r="R42" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C43" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="4" t="n">
@@ -2952,18 +2790,18 @@
       <c r="O43" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R43" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="44" s="2" spans="1:18">
+      <c r="R43" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C44" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I44" t="n">
+      <c r="I44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="4" t="n">
@@ -2978,18 +2816,18 @@
       <c r="O44" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R44" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="45" s="2" spans="1:18">
+      <c r="R44" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C45" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I45" t="n">
+      <c r="I45" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="4" t="n">
@@ -3004,18 +2842,18 @@
       <c r="O45" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R45" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="46" s="2" spans="1:18">
+      <c r="R45" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C46" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I46" t="n">
+      <c r="I46" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="4" t="n">
@@ -3030,18 +2868,18 @@
       <c r="O46" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R46" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="47" s="2" spans="1:18">
+      <c r="R46" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C47" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H47" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I47" t="n">
+      <c r="I47" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J47" s="4" t="n">
@@ -3056,18 +2894,18 @@
       <c r="O47" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R47" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="48" s="2" spans="1:18">
+      <c r="R47" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C48" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H48" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I48" t="n">
+      <c r="I48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J48" s="4" t="n">
@@ -3082,18 +2920,18 @@
       <c r="O48" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R48" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="49" s="2" spans="1:18">
+      <c r="R48" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C49" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I49" t="n">
+      <c r="I49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J49" s="4" t="n">
@@ -3108,18 +2946,18 @@
       <c r="O49" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R49" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="50" s="2" spans="1:18">
+      <c r="R49" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I50" t="n">
+      <c r="I50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J50" s="4" t="n">
@@ -3134,18 +2972,18 @@
       <c r="O50" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R50" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="51" s="2" spans="1:18">
+      <c r="R50" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C51" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="n">
+      <c r="I51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="4" t="n">
@@ -3160,18 +2998,18 @@
       <c r="O51" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R51" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="52" s="2" spans="1:18">
+      <c r="R51" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C52" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H52" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="n">
+      <c r="I52" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J52" s="4" t="n">
@@ -3186,18 +3024,18 @@
       <c r="O52" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R52" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="53" s="2" spans="1:18">
+      <c r="R52" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C53" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H53" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="n">
+      <c r="I53" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J53" s="4" t="n">
@@ -3212,18 +3050,18 @@
       <c r="O53" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R53" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="54" s="2" spans="1:18">
+      <c r="R53" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C54" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H54" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I54" t="n">
+      <c r="I54" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J54" s="4" t="n">
@@ -3238,18 +3076,18 @@
       <c r="O54" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R54" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="55" s="2" spans="1:18">
+      <c r="R54" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C55" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H55" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I55" t="n">
+      <c r="I55" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J55" s="4" t="n">
@@ -3264,18 +3102,18 @@
       <c r="O55" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R55" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.9" r="56" s="2" spans="1:18">
+      <c r="R55" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C56" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H56" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I56" t="n">
+      <c r="I56" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J56" s="4" t="n">
@@ -3290,57 +3128,63 @@
       <c r="O56" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R56" s="3" t="s">
+      <c r="R56" s="14" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule dxfId="3" priority="2" type="duplicateValues"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule dxfId="0" operator="notBetween" priority="3" type="cellIs">
+    <cfRule type="cellIs" priority="3" operator="notBetween" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>5.75</formula>
       <formula>6.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule dxfId="0" operator="notBetween" priority="4" type="cellIs">
+    <cfRule type="cellIs" priority="4" operator="notBetween" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>13000</formula>
       <formula>17000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule dxfId="0" operator="notBetween" priority="5" type="cellIs">
+    <cfRule type="cellIs" priority="5" operator="notBetween" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>545</formula>
       <formula>555</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="B4" activeCellId="2" sqref="R38:R56 R37 B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="R4:R36 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="10.5703125"/>
-    <col customWidth="1" max="2" min="2" style="2" width="29.7109375"/>
-    <col customWidth="1" max="1025" min="3" style="2" width="10.5703125"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="29.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="2" width="10.53"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="3" s="2" spans="1:3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="12" t="s">
         <v>39</v>
       </c>
@@ -3348,7 +3192,7 @@
         <v>10000919</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="2" spans="1:3">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
@@ -3357,7 +3201,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>